<commit_message>
large revision of classes and data
1) Cleaned up naming convention in classes + data.
2)  Separated model into heat and electricity markets (separate geographic indices)
3) Tested storage model.
Still to do: Add greenfield models.
</commit_message>
<xml_diff>
--- a/Data/mBasicInt.xlsx
+++ b/Data/mBasicInt.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\lpCompiler\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\EnergyEconomicsE2023\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="2" r:id="rId1"/>
@@ -547,7 +547,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -762,6 +762,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -852,6 +853,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -859,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,6 +893,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -975,6 +978,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1190,6 +1194,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1276,5 +1281,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated with material for lecture 3
</commit_message>
<xml_diff>
--- a/Data/mBasicInt.xlsx
+++ b/Data/mBasicInt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="2" r:id="rId1"/>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +771,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -880,7 +880,7 @@
         <v>59</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>